<commit_message>
margin and savefig config
</commit_message>
<xml_diff>
--- a/assets/bubble.xlsx
+++ b/assets/bubble.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheny\py\patentvis\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7218BE07-BDEC-45FC-8E0E-D4B6686F878A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C716F7A-6EA2-4008-931C-3F85C723845C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bubble" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>CD-SAXS</t>
   </si>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1009,11 +1010,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1113,5 +1114,114 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDE9E6B-3C85-4B4E-A8D8-5312FE621449}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>45</v>
+      </c>
+      <c r="D2">
+        <v>62</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>70</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>137</v>
+      </c>
+      <c r="C3">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>317</v>
+      </c>
+      <c r="G3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>43</v>
+      </c>
+      <c r="C4">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>102</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>87</v>
+      </c>
+      <c r="G4">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>